<commit_message>
Update lecturer id and name when user chooses to update timetable
Related Work Items: #1521
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B72031B-0693-436D-8772-B4943BDF28A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC98766F-40D5-4CFE-8C61-FAEB1CA1C4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9665" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9671" uniqueCount="865">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -6363,10 +6363,10 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F128" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P149" sqref="P149"/>
+      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6534,7 +6534,9 @@
       <c r="O2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="10"/>
+      <c r="P2" s="10" t="s">
+        <v>864</v>
+      </c>
       <c r="Q2" s="10" t="s">
         <v>43</v>
       </c>
@@ -6629,7 +6631,7 @@
         <v>59</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>60</v>
+        <v>864</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>61</v>
@@ -20440,9 +20442,7 @@
       <c r="O147" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="P147" s="8" t="s">
-        <v>864</v>
-      </c>
+      <c r="P147" s="8"/>
       <c r="Q147" s="8" t="s">
         <v>472</v>
       </c>

</xml_diff>

<commit_message>
Update progress bar when import timetable
Related Work Items: #1521
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB87869-3364-478B-B973-CE703AAA42C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3CC4E5-4532-4349-B68A-0AF144CD5153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5428,7 +5428,7 @@
     <t>197pm21905</t>
   </si>
   <si>
-    <t>Tên H</t>
+    <t>Tên HP</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
FIx bug during import
Related Work Items: #1521
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5046E80B-1E1A-49AD-8D5D-EFDBF3B60727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3285C800-E607-4625-9DF6-B7C7BFBAA7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9662" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9656" uniqueCount="873">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -6393,10 +6393,10 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="M307" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P25" sqref="P25"/>
+      <selection pane="bottomRight" activeCell="C318" sqref="C318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update progress bar while import lecturer and trim string
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3285C800-E607-4625-9DF6-B7C7BFBAA7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2E5177-5917-44D6-B694-6B8D07BC46AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9656" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9653" uniqueCount="874">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -5456,6 +5456,9 @@
   </si>
   <si>
     <t>197PM21905</t>
+  </si>
+  <si>
+    <t>ha</t>
   </si>
 </sst>
 </file>
@@ -6393,10 +6396,10 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="M307" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C318" sqref="C318"/>
+      <selection pane="bottomRight" activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6564,7 +6567,9 @@
       <c r="O2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="10"/>
+      <c r="P2" s="10" t="s">
+        <v>873</v>
+      </c>
       <c r="Q2" s="10" t="s">
         <v>43</v>
       </c>
@@ -7316,9 +7321,7 @@
       <c r="O10" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="P10" s="8" t="s">
-        <v>860</v>
-      </c>
+      <c r="P10" s="8"/>
       <c r="Q10" s="8" t="s">
         <v>92</v>
       </c>
@@ -7412,9 +7415,7 @@
       <c r="O11" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="8" t="s">
-        <v>860</v>
-      </c>
+      <c r="P11" s="8"/>
       <c r="Q11" s="8" t="s">
         <v>97</v>
       </c>
@@ -7508,9 +7509,7 @@
       <c r="O12" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="P12" s="8" t="s">
-        <v>860</v>
-      </c>
+      <c r="P12" s="8"/>
       <c r="Q12" s="8" t="s">
         <v>82</v>
       </c>
@@ -7604,9 +7603,7 @@
       <c r="O13" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="P13" s="8" t="s">
-        <v>860</v>
-      </c>
+      <c r="P13" s="8"/>
       <c r="Q13" s="8" t="s">
         <v>92</v>
       </c>
@@ -7700,9 +7697,7 @@
       <c r="O14" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="P14" s="8" t="s">
-        <v>860</v>
-      </c>
+      <c r="P14" s="8"/>
       <c r="Q14" s="8" t="s">
         <v>73</v>
       </c>
@@ -7796,9 +7791,7 @@
       <c r="O15" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P15" s="8" t="s">
-        <v>860</v>
-      </c>
+      <c r="P15" s="8"/>
       <c r="Q15" s="8" t="s">
         <v>73</v>
       </c>
@@ -7892,9 +7885,7 @@
       <c r="O16" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P16" s="8" t="s">
-        <v>860</v>
-      </c>
+      <c r="P16" s="8"/>
       <c r="Q16" s="8" t="s">
         <v>73</v>
       </c>
@@ -7988,9 +7979,7 @@
       <c r="O17" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="P17" s="8" t="s">
-        <v>860</v>
-      </c>
+      <c r="P17" s="8"/>
       <c r="Q17" s="8" t="s">
         <v>97</v>
       </c>
@@ -8084,9 +8073,7 @@
       <c r="O18" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="P18" s="8" t="s">
-        <v>860</v>
-      </c>
+      <c r="P18" s="8"/>
       <c r="Q18" s="8" t="s">
         <v>111</v>
       </c>
@@ -8180,9 +8167,7 @@
       <c r="O19" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="P19" s="8" t="s">
-        <v>860</v>
-      </c>
+      <c r="P19" s="8"/>
       <c r="Q19" s="8" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
Update re-import flow after import user
Related Work Items: #1521
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2E5177-5917-44D6-B694-6B8D07BC46AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E5DE8F-C84F-4366-AF2B-0CF6317D74A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1044" yWindow="2364" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TIÊU CHUẨN- phân công GV K28" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9653" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9647" uniqueCount="873">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -5456,9 +5456,6 @@
   </si>
   <si>
     <t>197PM21905</t>
-  </si>
-  <si>
-    <t>ha</t>
   </si>
 </sst>
 </file>
@@ -6396,10 +6393,10 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="L16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q12" sqref="Q12"/>
+      <selection pane="bottomRight" activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6568,7 +6565,7 @@
         <v>42</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>873</v>
+        <v>860</v>
       </c>
       <c r="Q2" s="10" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Update z-index of dropzone details
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E5DE8F-C84F-4366-AF2B-0CF6317D74A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA0057E-69E9-4E2A-B005-4D3DB57DE98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="2364" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TIÊU CHUẨN- phân công GV K28" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9647" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9646" uniqueCount="873">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -6393,10 +6393,10 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="L16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q28" sqref="Q28"/>
+      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6564,9 +6564,7 @@
       <c r="O2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="10" t="s">
-        <v>860</v>
-      </c>
+      <c r="P2" s="10"/>
       <c r="Q2" s="10" t="s">
         <v>43</v>
       </c>

</xml_diff>